<commit_message>
fix tempo chart x-axis
</commit_message>
<xml_diff>
--- a/Analysis/tempo/tempo chart.xlsx
+++ b/Analysis/tempo/tempo chart.xlsx
@@ -252,108 +252,6 @@
     <t>77 Akamul al-bha</t>
   </si>
   <si>
-    <t>77 Tushiyya</t>
-  </si>
-  <si>
-    <t>78 Allaylu layllu 'ajib</t>
-  </si>
-  <si>
-    <t>79 Ana qad 'aya sabri</t>
-  </si>
-  <si>
-    <t>80 Qalbi tarahu yafrah</t>
-  </si>
-  <si>
-    <t>81 Katamtu al-mahabbah sinin</t>
-  </si>
-  <si>
-    <t>82 Tushiyya (interlude)</t>
-  </si>
-  <si>
-    <t>83 Ya tal'a al-badri</t>
-  </si>
-  <si>
-    <t>84 Wa fi wisalika</t>
-  </si>
-  <si>
-    <t>85 Fadahta bil-muhayya</t>
-  </si>
-  <si>
-    <t>86 Nahwa mina al-ghizlan</t>
-  </si>
-  <si>
-    <t>87 al-Hubb 'sakruh abtal</t>
-  </si>
-  <si>
-    <t>88 Fi 'ishqati hara al-tibib</t>
-  </si>
-  <si>
-    <t>89 Yaquluna fi al-bustani</t>
-  </si>
-  <si>
-    <t>90 Wa muhafhafin</t>
-  </si>
-  <si>
-    <t>91 al-Laym la tlumni</t>
-  </si>
-  <si>
-    <t>92 Walaw annani</t>
-  </si>
-  <si>
-    <t>93 Kulla yawmin</t>
-  </si>
-  <si>
-    <t>94 Ya man idha aqbala</t>
-  </si>
-  <si>
-    <t>95 Tushiyya (interlude)</t>
-  </si>
-  <si>
-    <t>96 Ahin min law'a</t>
-  </si>
-  <si>
-    <t>97 Jad 'iliyya burdah</t>
-  </si>
-  <si>
-    <t>98 Tushiyya (interlude)</t>
-  </si>
-  <si>
-    <t>99 Aw hashta mud ghibta</t>
-  </si>
-  <si>
-    <t>100 Ayyaha al-sa'ilu</t>
-  </si>
-  <si>
-    <t>101 Salu taj al-mlah</t>
-  </si>
-  <si>
-    <t>102 Tushiyya (interlude)</t>
-  </si>
-  <si>
-    <t>103 Imshi ya rasula</t>
-  </si>
-  <si>
-    <t>104 Tushiyya (interlude)</t>
-  </si>
-  <si>
-    <t>105 Ya muqabil</t>
-  </si>
-  <si>
-    <t>106 Ya man malakni 'abda</t>
-  </si>
-  <si>
-    <t>107 Tayyahtani bayna al-anam</t>
-  </si>
-  <si>
-    <t>108 Qum tara al-rawda</t>
-  </si>
-  <si>
-    <t>109 Iktasa bal-jamal</t>
-  </si>
-  <si>
-    <t>110 Aya fadiha al-badri</t>
-  </si>
-  <si>
     <t>Movement</t>
   </si>
   <si>
@@ -370,6 +268,108 @@
   </si>
   <si>
     <t>al-Quddam</t>
+  </si>
+  <si>
+    <t>78 Tushiyya</t>
+  </si>
+  <si>
+    <t>79 Allaylu layllu 'ajib</t>
+  </si>
+  <si>
+    <t>80 Ana qad 'aya sabri</t>
+  </si>
+  <si>
+    <t>81 Qalbi tarahu yafrah</t>
+  </si>
+  <si>
+    <t>82 Katamtu al-mahabbah sinin</t>
+  </si>
+  <si>
+    <t>83 Tushiyya (interlude)</t>
+  </si>
+  <si>
+    <t>84 Ya tal'a al-badri</t>
+  </si>
+  <si>
+    <t>85 Wa fi wisalika</t>
+  </si>
+  <si>
+    <t>86 Fadahta bil-muhayya</t>
+  </si>
+  <si>
+    <t>87 Nahwa mina al-ghizlan</t>
+  </si>
+  <si>
+    <t>88 al-Hubb 'sakruh abtal</t>
+  </si>
+  <si>
+    <t>89 Fi 'ishqati hara al-tibib</t>
+  </si>
+  <si>
+    <t>90 Yaquluna fi al-bustani</t>
+  </si>
+  <si>
+    <t>91 Wa muhafhafin</t>
+  </si>
+  <si>
+    <t>92 al-Laym la tlumni</t>
+  </si>
+  <si>
+    <t>93 Walaw annani</t>
+  </si>
+  <si>
+    <t>94 Kulla yawmin</t>
+  </si>
+  <si>
+    <t>95 Ya man idha aqbala</t>
+  </si>
+  <si>
+    <t>96 Tushiyya (interlude)</t>
+  </si>
+  <si>
+    <t>97 Ahin min law'a</t>
+  </si>
+  <si>
+    <t>98 Jad 'iliyya burdah</t>
+  </si>
+  <si>
+    <t>99 Tushiyya (interlude)</t>
+  </si>
+  <si>
+    <t>100 Aw hashta mud ghibta</t>
+  </si>
+  <si>
+    <t>101 Ayyaha al-sa'ilu</t>
+  </si>
+  <si>
+    <t>102 Salu taj al-mlah</t>
+  </si>
+  <si>
+    <t>103 Tushiyya (interlude)</t>
+  </si>
+  <si>
+    <t>104 Imshi ya rasula</t>
+  </si>
+  <si>
+    <t>105 Tushiyya (interlude)</t>
+  </si>
+  <si>
+    <t>106 Ya muqabil</t>
+  </si>
+  <si>
+    <t>107 Ya man malakni 'abda</t>
+  </si>
+  <si>
+    <t>108 Tayyahtani bayna al-anam</t>
+  </si>
+  <si>
+    <t>109 Qum tara al-rawda</t>
+  </si>
+  <si>
+    <t>110 Iktasa bal-jamal</t>
+  </si>
+  <si>
+    <t>111 Aya fadiha al-badri</t>
   </si>
 </sst>
 </file>
@@ -418,8 +418,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -442,7 +446,7 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="23">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -452,6 +456,8 @@
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -461,6 +467,8 @@
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -489,28 +497,20 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr>
-                <a:latin typeface="Verdana"/>
-              </a:defRPr>
+              <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US">
-                <a:latin typeface="Verdana"/>
-              </a:rPr>
-              <a:t>Tempo </a:t>
+              <a:rPr lang="en-US"/>
+              <a:t>Tempo</a:t>
             </a:r>
           </a:p>
           <a:p>
             <a:pPr>
-              <a:defRPr>
-                <a:latin typeface="Verdana"/>
-              </a:defRPr>
+              <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" b="0">
-                <a:latin typeface="Verdana"/>
-              </a:rPr>
-              <a:t>(BPM, adjusted for metric changes within movements)</a:t>
+              <a:rPr lang="en-US" b="0"/>
+              <a:t>(BPM, adjusted to account for metric changes)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -769,106 +769,106 @@
                   <c:v>77 Akamul al-bha</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>77 Tushiyya</c:v>
+                  <c:v>78 Tushiyya</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>78 Allaylu layllu 'ajib</c:v>
+                  <c:v>79 Allaylu layllu 'ajib</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>79 Ana qad 'aya sabri</c:v>
+                  <c:v>80 Ana qad 'aya sabri</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>80 Qalbi tarahu yafrah</c:v>
+                  <c:v>81 Qalbi tarahu yafrah</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>81 Katamtu al-mahabbah sinin</c:v>
+                  <c:v>82 Katamtu al-mahabbah sinin</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>82 Tushiyya (interlude)</c:v>
+                  <c:v>83 Tushiyya (interlude)</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>83 Ya tal'a al-badri</c:v>
+                  <c:v>84 Ya tal'a al-badri</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>84 Wa fi wisalika</c:v>
+                  <c:v>85 Wa fi wisalika</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>85 Fadahta bil-muhayya</c:v>
+                  <c:v>86 Fadahta bil-muhayya</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>86 Nahwa mina al-ghizlan</c:v>
+                  <c:v>87 Nahwa mina al-ghizlan</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>87 al-Hubb 'sakruh abtal</c:v>
+                  <c:v>88 al-Hubb 'sakruh abtal</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>88 Fi 'ishqati hara al-tibib</c:v>
+                  <c:v>89 Fi 'ishqati hara al-tibib</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>89 Yaquluna fi al-bustani</c:v>
+                  <c:v>90 Yaquluna fi al-bustani</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>90 Wa muhafhafin</c:v>
+                  <c:v>91 Wa muhafhafin</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>91 al-Laym la tlumni</c:v>
+                  <c:v>92 al-Laym la tlumni</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>92 Walaw annani</c:v>
+                  <c:v>93 Walaw annani</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>93 Kulla yawmin</c:v>
+                  <c:v>94 Kulla yawmin</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>94 Ya man idha aqbala</c:v>
+                  <c:v>95 Ya man idha aqbala</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>95 Tushiyya (interlude)</c:v>
+                  <c:v>96 Tushiyya (interlude)</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>96 Ahin min law'a</c:v>
+                  <c:v>97 Ahin min law'a</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>97 Jad 'iliyya burdah</c:v>
+                  <c:v>98 Jad 'iliyya burdah</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>98 Tushiyya (interlude)</c:v>
+                  <c:v>99 Tushiyya (interlude)</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>99 Aw hashta mud ghibta</c:v>
+                  <c:v>100 Aw hashta mud ghibta</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>100 Ayyaha al-sa'ilu</c:v>
+                  <c:v>101 Ayyaha al-sa'ilu</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>101 Salu taj al-mlah</c:v>
+                  <c:v>102 Salu taj al-mlah</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>102 Tushiyya (interlude)</c:v>
+                  <c:v>103 Tushiyya (interlude)</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>103 Imshi ya rasula</c:v>
+                  <c:v>104 Imshi ya rasula</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>104 Tushiyya (interlude)</c:v>
+                  <c:v>105 Tushiyya (interlude)</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>105 Ya muqabil</c:v>
+                  <c:v>106 Ya muqabil</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>106 Ya man malakni 'abda</c:v>
+                  <c:v>107 Ya man malakni 'abda</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>107 Tayyahtani bayna al-anam</c:v>
+                  <c:v>108 Tayyahtani bayna al-anam</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>108 Qum tara al-rawda</c:v>
+                  <c:v>109 Qum tara al-rawda</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>109 Iktasa bal-jamal</c:v>
+                  <c:v>110 Iktasa bal-jamal</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>110 Aya fadiha al-badri</c:v>
+                  <c:v>111 Aya fadiha al-badri</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1218,11 +1218,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2056672664"/>
-        <c:axId val="2056675752"/>
+        <c:axId val="2105149272"/>
+        <c:axId val="2119139624"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2056672664"/>
+        <c:axId val="2105149272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1231,7 +1231,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2056675752"/>
+        <c:crossAx val="2119139624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1239,7 +1239,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2056675752"/>
+        <c:axId val="2119139624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1250,7 +1250,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2056672664"/>
+        <c:crossAx val="2105149272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1277,19 +1277,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:colOff>139700</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>482600</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>622300</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1631,8 +1631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DE5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2193,106 +2193,106 @@
         <v>76</v>
       </c>
       <c r="BX2" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="BY2" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="BZ2" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="CA2" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="CB2" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="CC2" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="CD2" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="CE2" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="CF2" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="CG2" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="CH2" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="CI2" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="CJ2" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="CK2" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="CL2" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="CM2" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="CN2" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="CO2" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="CP2" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="CQ2" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="CR2" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="CS2" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="CT2" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="CU2" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="CV2" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="CW2" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="CX2" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="CY2" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="CZ2" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="DA2" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="DB2" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="DC2" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="DD2" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="DE2" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:109">
@@ -2431,11 +2431,11 @@
         <v>104</v>
       </c>
       <c r="AR3">
-        <f>AR5*2</f>
+        <f t="shared" ref="AR3:BC3" si="1">AR5*2</f>
         <v>152</v>
       </c>
       <c r="AS3">
-        <f t="shared" ref="AS3:BC3" si="1">AS5*2</f>
+        <f t="shared" si="1"/>
         <v>168</v>
       </c>
       <c r="AT3">
@@ -2620,11 +2620,11 @@
         <v>92</v>
       </c>
       <c r="CY3">
-        <f>CY5*2</f>
+        <f t="shared" ref="CY3:DE3" si="2">CY5*2</f>
         <v>138</v>
       </c>
       <c r="CZ3">
-        <f t="shared" ref="CZ3:DE3" si="2">CZ5*2</f>
+        <f t="shared" si="2"/>
         <v>138</v>
       </c>
       <c r="DA3">
@@ -2650,331 +2650,331 @@
     </row>
     <row r="4" spans="1:109">
       <c r="A4" t="s">
-        <v>111</v>
+        <v>77</v>
       </c>
       <c r="B4" t="s">
-        <v>112</v>
+        <v>78</v>
       </c>
       <c r="C4" t="s">
-        <v>112</v>
+        <v>78</v>
       </c>
       <c r="D4" t="s">
-        <v>112</v>
+        <v>78</v>
       </c>
       <c r="E4" t="s">
-        <v>112</v>
+        <v>78</v>
       </c>
       <c r="F4" t="s">
-        <v>112</v>
+        <v>78</v>
       </c>
       <c r="G4" t="s">
-        <v>112</v>
+        <v>78</v>
       </c>
       <c r="H4" t="s">
-        <v>112</v>
+        <v>78</v>
       </c>
       <c r="I4" t="s">
-        <v>112</v>
+        <v>78</v>
       </c>
       <c r="J4" t="s">
-        <v>112</v>
+        <v>78</v>
       </c>
       <c r="K4" t="s">
-        <v>112</v>
+        <v>78</v>
       </c>
       <c r="L4" t="s">
-        <v>112</v>
+        <v>78</v>
       </c>
       <c r="M4" t="s">
-        <v>112</v>
+        <v>78</v>
       </c>
       <c r="N4" t="s">
-        <v>113</v>
+        <v>79</v>
       </c>
       <c r="O4" t="s">
-        <v>113</v>
+        <v>79</v>
       </c>
       <c r="P4" t="s">
-        <v>113</v>
+        <v>79</v>
       </c>
       <c r="Q4" t="s">
-        <v>113</v>
+        <v>79</v>
       </c>
       <c r="R4" t="s">
-        <v>113</v>
+        <v>79</v>
       </c>
       <c r="S4" t="s">
-        <v>113</v>
+        <v>79</v>
       </c>
       <c r="T4" t="s">
-        <v>113</v>
+        <v>79</v>
       </c>
       <c r="U4" t="s">
-        <v>113</v>
+        <v>79</v>
       </c>
       <c r="V4" t="s">
-        <v>113</v>
+        <v>79</v>
       </c>
       <c r="W4" t="s">
-        <v>113</v>
+        <v>79</v>
       </c>
       <c r="X4" t="s">
-        <v>113</v>
+        <v>79</v>
       </c>
       <c r="Y4" t="s">
-        <v>113</v>
+        <v>79</v>
       </c>
       <c r="Z4" t="s">
-        <v>113</v>
+        <v>79</v>
       </c>
       <c r="AA4" t="s">
-        <v>113</v>
+        <v>79</v>
       </c>
       <c r="AB4" t="s">
-        <v>113</v>
+        <v>79</v>
       </c>
       <c r="AC4" t="s">
-        <v>113</v>
+        <v>79</v>
       </c>
       <c r="AD4" t="s">
-        <v>113</v>
+        <v>79</v>
       </c>
       <c r="AE4" t="s">
-        <v>114</v>
+        <v>80</v>
       </c>
       <c r="AF4" t="s">
-        <v>114</v>
+        <v>80</v>
       </c>
       <c r="AG4" t="s">
-        <v>114</v>
+        <v>80</v>
       </c>
       <c r="AH4" t="s">
-        <v>114</v>
+        <v>80</v>
       </c>
       <c r="AI4" t="s">
-        <v>114</v>
+        <v>80</v>
       </c>
       <c r="AJ4" t="s">
-        <v>114</v>
+        <v>80</v>
       </c>
       <c r="AK4" t="s">
-        <v>114</v>
+        <v>80</v>
       </c>
       <c r="AL4" t="s">
-        <v>114</v>
+        <v>80</v>
       </c>
       <c r="AM4" t="s">
-        <v>114</v>
+        <v>80</v>
       </c>
       <c r="AN4" t="s">
-        <v>114</v>
+        <v>80</v>
       </c>
       <c r="AO4" t="s">
-        <v>114</v>
+        <v>80</v>
       </c>
       <c r="AP4" t="s">
-        <v>114</v>
+        <v>80</v>
       </c>
       <c r="AQ4" t="s">
-        <v>114</v>
+        <v>80</v>
       </c>
       <c r="AR4" t="s">
-        <v>114</v>
+        <v>80</v>
       </c>
       <c r="AS4" t="s">
-        <v>114</v>
+        <v>80</v>
       </c>
       <c r="AT4" t="s">
-        <v>114</v>
+        <v>80</v>
       </c>
       <c r="AU4" t="s">
-        <v>114</v>
+        <v>80</v>
       </c>
       <c r="AV4" t="s">
-        <v>114</v>
+        <v>80</v>
       </c>
       <c r="AW4" t="s">
-        <v>114</v>
+        <v>80</v>
       </c>
       <c r="AX4" t="s">
-        <v>114</v>
+        <v>80</v>
       </c>
       <c r="AY4" t="s">
-        <v>114</v>
+        <v>80</v>
       </c>
       <c r="AZ4" t="s">
-        <v>114</v>
+        <v>80</v>
       </c>
       <c r="BA4" t="s">
-        <v>114</v>
+        <v>80</v>
       </c>
       <c r="BB4" t="s">
-        <v>114</v>
+        <v>80</v>
       </c>
       <c r="BC4" t="s">
-        <v>114</v>
+        <v>80</v>
       </c>
       <c r="BD4" t="s">
-        <v>115</v>
+        <v>81</v>
       </c>
       <c r="BE4" t="s">
-        <v>115</v>
+        <v>81</v>
       </c>
       <c r="BF4" t="s">
-        <v>115</v>
+        <v>81</v>
       </c>
       <c r="BG4" t="s">
-        <v>115</v>
+        <v>81</v>
       </c>
       <c r="BH4" t="s">
-        <v>115</v>
+        <v>81</v>
       </c>
       <c r="BI4" t="s">
-        <v>115</v>
+        <v>81</v>
       </c>
       <c r="BJ4" t="s">
-        <v>115</v>
+        <v>81</v>
       </c>
       <c r="BK4" t="s">
-        <v>115</v>
+        <v>81</v>
       </c>
       <c r="BL4" t="s">
-        <v>115</v>
+        <v>81</v>
       </c>
       <c r="BM4" t="s">
-        <v>115</v>
+        <v>81</v>
       </c>
       <c r="BN4" t="s">
-        <v>115</v>
+        <v>81</v>
       </c>
       <c r="BO4" t="s">
-        <v>115</v>
+        <v>81</v>
       </c>
       <c r="BP4" t="s">
-        <v>115</v>
+        <v>81</v>
       </c>
       <c r="BQ4" t="s">
-        <v>115</v>
+        <v>81</v>
       </c>
       <c r="BR4" t="s">
-        <v>115</v>
+        <v>81</v>
       </c>
       <c r="BS4" t="s">
-        <v>115</v>
+        <v>81</v>
       </c>
       <c r="BT4" t="s">
-        <v>115</v>
+        <v>81</v>
       </c>
       <c r="BU4" t="s">
-        <v>115</v>
+        <v>81</v>
       </c>
       <c r="BV4" t="s">
-        <v>115</v>
+        <v>81</v>
       </c>
       <c r="BW4" t="s">
-        <v>115</v>
+        <v>81</v>
       </c>
       <c r="BX4" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
       <c r="BY4" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
       <c r="BZ4" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
       <c r="CA4" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
       <c r="CB4" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
       <c r="CC4" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
       <c r="CD4" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
       <c r="CE4" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
       <c r="CF4" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
       <c r="CG4" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
       <c r="CH4" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
       <c r="CI4" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
       <c r="CJ4" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
       <c r="CK4" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
       <c r="CL4" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
       <c r="CM4" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
       <c r="CN4" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
       <c r="CO4" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
       <c r="CP4" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
       <c r="CQ4" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
       <c r="CR4" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
       <c r="CS4" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
       <c r="CT4" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
       <c r="CU4" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
       <c r="CV4" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
       <c r="CW4" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
       <c r="CX4" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
       <c r="CY4" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
       <c r="CZ4" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
       <c r="DA4" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
       <c r="DB4" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
       <c r="DC4" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
       <c r="DD4" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
       <c r="DE4" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:109">

</xml_diff>

<commit_message>
function to find specific motives (contour only)
</commit_message>
<xml_diff>
--- a/Analysis/tempo/tempo chart.xlsx
+++ b/Analysis/tempo/tempo chart.xlsx
@@ -382,6 +382,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -543,9 +544,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'tempo chart.csv'!$B$2:$DE$2</c:f>
+              <c:f>'tempo chart.csv'!$B$2:$DI$2</c:f>
               <c:strCache>
-                <c:ptCount val="108"/>
+                <c:ptCount val="112"/>
                 <c:pt idx="0">
                   <c:v>3 Tushiyya</c:v>
                 </c:pt>
@@ -582,292 +583,292 @@
                 <c:pt idx="11">
                   <c:v>15 Hadha al-nahar</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>16 Tushiyya</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>17 Mahma nara</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>18 Ya laylu tul</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>19 Law rahu iblis</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>20 Law laka ma himtu wajda</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>21 Hal tusta'adu ayyamuna</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>22 Bidha al-hubb n'ammar qalbi</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>23 Hubbu al-habib</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>24 Al-shawqu 'allumni al-sahar</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>25 Tayyahtani bayna al-anam</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>26 Lamma bada minka al-qabul</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>27 Atani mina al-khuldi</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>28 Qalbi yakhaf</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>29 Bada'i'u al-husni</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>30 Inna al-muluka</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="28">
                   <c:v>31 Ya sura qamar</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="29">
                   <c:v>32 Wa nashkuru fi dha al-maqam</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="31">
                   <c:v>33 Tushiyya</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="32">
                   <c:v>34 Lamu al-'idhari</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="33">
                   <c:v>35 Abshir bil-hana</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="34">
                   <c:v>36 Allah Ya Rabbi</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="35">
                   <c:v>37 Hal tusta'adu ayyamuna bil-khaliji</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="36">
                   <c:v>38 Bi-Allah ya tabiba al-hawa</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="37">
                   <c:v>39 Binta</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="38">
                   <c:v>40 Qam min nu'asuh</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="39">
                   <c:v>41 'Aqaribu al-Asdhagh</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="40">
                   <c:v>42 Malihu al-Muhayya</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="41">
                   <c:v>43 Qalbi Hasal</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="42">
                   <c:v>44 Ya qalbi bushra</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="43">
                   <c:v>45 Ma'ani al-Hawa</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="44">
                   <c:v>46 Umna' raqadi</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="45">
                   <c:v>47 Ya qalbi tasabbar</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="46">
                   <c:v>48 Ma ladhdhatu al-furjah</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="47">
                   <c:v>49 Nahwa mina al-ghizlan</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="48">
                   <c:v>50 Law laka ma himtu wajda</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="49">
                   <c:v>51 Ya 'ajbi</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="50">
                   <c:v>52 Ihtakam fiyya</c:v>
                 </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="51">
                   <c:v>53 Ya nadimi</c:v>
                 </c:pt>
-                <c:pt idx="50">
+                <c:pt idx="52">
                   <c:v>54 Faha al-banafsaj</c:v>
                 </c:pt>
-                <c:pt idx="51">
+                <c:pt idx="53">
                   <c:v>55 Hubbik amira al-milah</c:v>
                 </c:pt>
-                <c:pt idx="52">
+                <c:pt idx="54">
                   <c:v>56 Nahwa al-hajiba al-akhal</c:v>
                 </c:pt>
-                <c:pt idx="53">
+                <c:pt idx="55">
                   <c:v>57 Sahib mabsam</c:v>
                 </c:pt>
-                <c:pt idx="54">
+                <c:pt idx="57">
                   <c:v>58 Buh bil-ghara mi</c:v>
                 </c:pt>
-                <c:pt idx="55">
+                <c:pt idx="58">
                   <c:v>59 Fiq ya nadim</c:v>
                 </c:pt>
-                <c:pt idx="56">
+                <c:pt idx="59">
                   <c:v>60 Man malak 'aqli rahin</c:v>
                 </c:pt>
-                <c:pt idx="57">
+                <c:pt idx="60">
                   <c:v>61 Qad zara man nahwah</c:v>
                 </c:pt>
-                <c:pt idx="58">
+                <c:pt idx="61">
                   <c:v>62 Umun lam</c:v>
                 </c:pt>
-                <c:pt idx="59">
+                <c:pt idx="62">
                   <c:v>63 Ahi 'ala sa'a</c:v>
                 </c:pt>
-                <c:pt idx="60">
+                <c:pt idx="63">
                   <c:v>64 Ya sa'd min a'tah</c:v>
                 </c:pt>
-                <c:pt idx="61">
+                <c:pt idx="64">
                   <c:v>65 Jami' man dkhal</c:v>
                 </c:pt>
-                <c:pt idx="62">
+                <c:pt idx="65">
                   <c:v>66 Ya malih</c:v>
                 </c:pt>
-                <c:pt idx="63">
+                <c:pt idx="66">
                   <c:v>67 Qalbi yakhaf mina al-gharam</c:v>
                 </c:pt>
-                <c:pt idx="64">
+                <c:pt idx="67">
                   <c:v>68 Ya al-'akfa fi smawi</c:v>
                 </c:pt>
-                <c:pt idx="65">
+                <c:pt idx="68">
                   <c:v>69 Law kan shawqi</c:v>
                 </c:pt>
-                <c:pt idx="66">
+                <c:pt idx="69">
                   <c:v>70 Inna wajdi</c:v>
                 </c:pt>
-                <c:pt idx="67">
+                <c:pt idx="70">
                   <c:v>71 Ya da'ifa al-jufun</c:v>
                 </c:pt>
-                <c:pt idx="68">
+                <c:pt idx="71">
                   <c:v>72 Ghazal</c:v>
                 </c:pt>
-                <c:pt idx="69">
+                <c:pt idx="72">
                   <c:v>73 Kullu shay lahu antiha' wahadu</c:v>
                 </c:pt>
-                <c:pt idx="70">
+                <c:pt idx="73">
                   <c:v>74 Afdi ghazalan</c:v>
                 </c:pt>
-                <c:pt idx="71">
+                <c:pt idx="74">
                   <c:v>75 Qalbi tmkan bal-nadhra</c:v>
                 </c:pt>
-                <c:pt idx="72">
+                <c:pt idx="75">
                   <c:v>76 Fi wasfihi al-asna</c:v>
                 </c:pt>
-                <c:pt idx="73">
+                <c:pt idx="76">
                   <c:v>77 Akamul al-bha</c:v>
                 </c:pt>
-                <c:pt idx="74">
+                <c:pt idx="78">
                   <c:v>78 Tushiyya</c:v>
                 </c:pt>
-                <c:pt idx="75">
+                <c:pt idx="79">
                   <c:v>79 Allaylu layllu 'ajib</c:v>
                 </c:pt>
-                <c:pt idx="76">
+                <c:pt idx="80">
                   <c:v>80 Ana qad 'aya sabri</c:v>
                 </c:pt>
-                <c:pt idx="77">
+                <c:pt idx="81">
                   <c:v>81 Qalbi tarahu yafrah</c:v>
                 </c:pt>
-                <c:pt idx="78">
+                <c:pt idx="82">
                   <c:v>82 Katamtu al-mahabbah sinin</c:v>
                 </c:pt>
-                <c:pt idx="79">
+                <c:pt idx="83">
                   <c:v>83 Tushiyya (interlude)</c:v>
                 </c:pt>
-                <c:pt idx="80">
+                <c:pt idx="84">
                   <c:v>84 Ya tal'a al-badri</c:v>
                 </c:pt>
-                <c:pt idx="81">
+                <c:pt idx="85">
                   <c:v>85 Wa fi wisalika</c:v>
                 </c:pt>
-                <c:pt idx="82">
+                <c:pt idx="86">
                   <c:v>86 Fadahta bil-muhayya</c:v>
                 </c:pt>
-                <c:pt idx="83">
+                <c:pt idx="87">
                   <c:v>87 Nahwa mina al-ghizlan</c:v>
                 </c:pt>
-                <c:pt idx="84">
+                <c:pt idx="88">
                   <c:v>88 al-Hubb 'sakruh abtal</c:v>
                 </c:pt>
-                <c:pt idx="85">
+                <c:pt idx="89">
                   <c:v>89 Fi 'ishqati hara al-tibib</c:v>
                 </c:pt>
-                <c:pt idx="86">
+                <c:pt idx="90">
                   <c:v>90 Yaquluna fi al-bustani</c:v>
                 </c:pt>
-                <c:pt idx="87">
+                <c:pt idx="91">
                   <c:v>91 Wa muhafhafin</c:v>
                 </c:pt>
-                <c:pt idx="88">
+                <c:pt idx="92">
                   <c:v>92 al-Laym la tlumni</c:v>
                 </c:pt>
-                <c:pt idx="89">
+                <c:pt idx="93">
                   <c:v>93 Walaw annani</c:v>
                 </c:pt>
-                <c:pt idx="90">
+                <c:pt idx="94">
                   <c:v>94 Kulla yawmin</c:v>
                 </c:pt>
-                <c:pt idx="91">
+                <c:pt idx="95">
                   <c:v>95 Ya man idha aqbala</c:v>
                 </c:pt>
-                <c:pt idx="92">
+                <c:pt idx="96">
                   <c:v>96 Tushiyya (interlude)</c:v>
                 </c:pt>
-                <c:pt idx="93">
+                <c:pt idx="97">
                   <c:v>97 Ahin min law'a</c:v>
                 </c:pt>
-                <c:pt idx="94">
+                <c:pt idx="98">
                   <c:v>98 Jad 'iliyya burdah</c:v>
                 </c:pt>
-                <c:pt idx="95">
+                <c:pt idx="99">
                   <c:v>99 Tushiyya (interlude)</c:v>
                 </c:pt>
-                <c:pt idx="96">
+                <c:pt idx="100">
                   <c:v>100 Aw hashta mud ghibta</c:v>
                 </c:pt>
-                <c:pt idx="97">
+                <c:pt idx="101">
                   <c:v>101 Ayyaha al-sa'ilu</c:v>
                 </c:pt>
-                <c:pt idx="98">
+                <c:pt idx="102">
                   <c:v>102 Salu taj al-mlah</c:v>
                 </c:pt>
-                <c:pt idx="99">
+                <c:pt idx="103">
                   <c:v>103 Tushiyya (interlude)</c:v>
                 </c:pt>
-                <c:pt idx="100">
+                <c:pt idx="104">
                   <c:v>104 Imshi ya rasula</c:v>
                 </c:pt>
-                <c:pt idx="101">
+                <c:pt idx="105">
                   <c:v>105 Tushiyya (interlude)</c:v>
                 </c:pt>
-                <c:pt idx="102">
+                <c:pt idx="106">
                   <c:v>106 Ya muqabil</c:v>
                 </c:pt>
-                <c:pt idx="103">
+                <c:pt idx="107">
                   <c:v>107 Ya man malakni 'abda</c:v>
                 </c:pt>
-                <c:pt idx="104">
+                <c:pt idx="108">
                   <c:v>108 Tayyahtani bayna al-anam</c:v>
                 </c:pt>
-                <c:pt idx="105">
+                <c:pt idx="109">
                   <c:v>109 Qum tara al-rawda</c:v>
                 </c:pt>
-                <c:pt idx="106">
+                <c:pt idx="110">
                   <c:v>110 Iktasa bal-jamal</c:v>
                 </c:pt>
-                <c:pt idx="107">
+                <c:pt idx="111">
                   <c:v>111 Aya fadiha al-badri</c:v>
                 </c:pt>
               </c:strCache>
@@ -875,10 +876,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'tempo chart.csv'!$B$3:$DE$3</c:f>
+              <c:f>'tempo chart.csv'!$B$3:$DI$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="108"/>
+                <c:ptCount val="112"/>
                 <c:pt idx="0">
                   <c:v>58.0</c:v>
                 </c:pt>
@@ -915,29 +916,26 @@
                 <c:pt idx="11">
                   <c:v>132.0</c:v>
                 </c:pt>
-                <c:pt idx="12">
-                  <c:v>72.0</c:v>
-                </c:pt>
                 <c:pt idx="13">
                   <c:v>72.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>78.0</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>80.0</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>84.0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>92.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>92.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>96.0</c:v>
+                  <c:v>92.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>96.0</c:v>
@@ -949,118 +947,112 @@
                   <c:v>96.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
+                  <c:v>96.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
                   <c:v>104.0</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>160.0</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>152.0</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>160.0</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="28">
                   <c:v>184.0</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="29">
                   <c:v>192.0</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>66.0</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>66.0</c:v>
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>66.0</c:v>
                 </c:pt>
                 <c:pt idx="32">
+                  <c:v>66.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>66.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
                   <c:v>72.0</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="35">
                   <c:v>72.0</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="36">
                   <c:v>80.0</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="37">
                   <c:v>84.0</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="38">
                   <c:v>88.0</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="39">
                   <c:v>92.0</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="40">
                   <c:v>96.0</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="41">
                   <c:v>100.0</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="42">
                   <c:v>100.0</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="43">
                   <c:v>104.0</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="44">
                   <c:v>152.0</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="45">
                   <c:v>168.0</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="46">
                   <c:v>184.0</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="47">
                   <c:v>192.0</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="48">
                   <c:v>192.0</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="49">
                   <c:v>208.0</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="50">
                   <c:v>208.0</c:v>
                 </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="51">
                   <c:v>216.0</c:v>
                 </c:pt>
-                <c:pt idx="50">
+                <c:pt idx="52">
                   <c:v>216.0</c:v>
                 </c:pt>
-                <c:pt idx="51">
+                <c:pt idx="53">
                   <c:v>224.0</c:v>
                 </c:pt>
-                <c:pt idx="52">
+                <c:pt idx="54">
                   <c:v>224.0</c:v>
                 </c:pt>
-                <c:pt idx="53">
+                <c:pt idx="55">
                   <c:v>232.0</c:v>
                 </c:pt>
-                <c:pt idx="54">
+                <c:pt idx="57">
                   <c:v>60.0</c:v>
                 </c:pt>
-                <c:pt idx="55">
+                <c:pt idx="58">
                   <c:v>63.0</c:v>
                 </c:pt>
-                <c:pt idx="56">
+                <c:pt idx="59">
                   <c:v>69.0</c:v>
                 </c:pt>
-                <c:pt idx="57">
+                <c:pt idx="60">
                   <c:v>72.0</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>76.0</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>76.0</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>76.0</c:v>
                 </c:pt>
                 <c:pt idx="61">
                   <c:v>76.0</c:v>
@@ -1072,76 +1064,73 @@
                   <c:v>76.0</c:v>
                 </c:pt>
                 <c:pt idx="64">
+                  <c:v>76.0</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>76.0</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>76.0</c:v>
+                </c:pt>
+                <c:pt idx="67">
                   <c:v>80.0</c:v>
                 </c:pt>
-                <c:pt idx="65">
+                <c:pt idx="68">
                   <c:v>80.0</c:v>
                 </c:pt>
-                <c:pt idx="66">
+                <c:pt idx="69">
                   <c:v>80.0</c:v>
                 </c:pt>
-                <c:pt idx="67">
+                <c:pt idx="70">
                   <c:v>84.0</c:v>
                 </c:pt>
-                <c:pt idx="68">
+                <c:pt idx="71">
                   <c:v>88.0</c:v>
                 </c:pt>
-                <c:pt idx="69">
+                <c:pt idx="72">
                   <c:v>96.0</c:v>
                 </c:pt>
-                <c:pt idx="70">
+                <c:pt idx="73">
                   <c:v>100.0</c:v>
                 </c:pt>
-                <c:pt idx="71">
+                <c:pt idx="74">
                   <c:v>104.0</c:v>
                 </c:pt>
-                <c:pt idx="72">
+                <c:pt idx="75">
                   <c:v>108.0</c:v>
                 </c:pt>
-                <c:pt idx="73">
+                <c:pt idx="76">
                   <c:v>126.0</c:v>
                 </c:pt>
-                <c:pt idx="74">
+                <c:pt idx="78">
                   <c:v>60.0</c:v>
                 </c:pt>
-                <c:pt idx="75">
+                <c:pt idx="79">
                   <c:v>63.0</c:v>
                 </c:pt>
-                <c:pt idx="76">
+                <c:pt idx="80">
                   <c:v>63.0</c:v>
                 </c:pt>
-                <c:pt idx="77">
+                <c:pt idx="81">
                   <c:v>66.0</c:v>
                 </c:pt>
-                <c:pt idx="78">
+                <c:pt idx="82">
                   <c:v>66.0</c:v>
                 </c:pt>
-                <c:pt idx="79">
+                <c:pt idx="83">
                   <c:v>69.0</c:v>
                 </c:pt>
-                <c:pt idx="80">
+                <c:pt idx="84">
                   <c:v>69.0</c:v>
                 </c:pt>
-                <c:pt idx="81">
+                <c:pt idx="85">
                   <c:v>69.0</c:v>
                 </c:pt>
-                <c:pt idx="82">
+                <c:pt idx="86">
                   <c:v>72.0</c:v>
                 </c:pt>
-                <c:pt idx="83">
+                <c:pt idx="87">
                   <c:v>72.0</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>76.0</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>76.0</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>76.0</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>76.0</c:v>
                 </c:pt>
                 <c:pt idx="88">
                   <c:v>76.0</c:v>
@@ -1162,45 +1151,57 @@
                   <c:v>76.0</c:v>
                 </c:pt>
                 <c:pt idx="94">
+                  <c:v>76.0</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>76.0</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>76.0</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>76.0</c:v>
+                </c:pt>
+                <c:pt idx="98">
                   <c:v>80.0</c:v>
                 </c:pt>
-                <c:pt idx="95">
+                <c:pt idx="99">
                   <c:v>80.0</c:v>
                 </c:pt>
-                <c:pt idx="96">
+                <c:pt idx="100">
                   <c:v>80.0</c:v>
                 </c:pt>
-                <c:pt idx="97">
+                <c:pt idx="101">
                   <c:v>84.0</c:v>
                 </c:pt>
-                <c:pt idx="98">
+                <c:pt idx="102">
                   <c:v>92.0</c:v>
                 </c:pt>
-                <c:pt idx="99">
+                <c:pt idx="103">
                   <c:v>92.0</c:v>
                 </c:pt>
-                <c:pt idx="100">
+                <c:pt idx="104">
                   <c:v>92.0</c:v>
                 </c:pt>
-                <c:pt idx="101">
+                <c:pt idx="105">
                   <c:v>138.0</c:v>
                 </c:pt>
-                <c:pt idx="102">
+                <c:pt idx="106">
                   <c:v>138.0</c:v>
                 </c:pt>
-                <c:pt idx="103">
+                <c:pt idx="107">
                   <c:v>156.0</c:v>
                 </c:pt>
-                <c:pt idx="104">
+                <c:pt idx="108">
                   <c:v>180.0</c:v>
                 </c:pt>
-                <c:pt idx="105">
+                <c:pt idx="109">
                   <c:v>198.0</c:v>
                 </c:pt>
-                <c:pt idx="106">
+                <c:pt idx="110">
                   <c:v>206.0</c:v>
                 </c:pt>
-                <c:pt idx="107">
+                <c:pt idx="111">
                   <c:v>216.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1218,11 +1219,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2105149272"/>
-        <c:axId val="2119139624"/>
+        <c:axId val="-2144380568"/>
+        <c:axId val="2118258888"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2105149272"/>
+        <c:axId val="-2144380568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1231,7 +1232,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2119139624"/>
+        <c:crossAx val="2118258888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1239,7 +1240,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2119139624"/>
+        <c:axId val="2118258888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1250,16 +1251,11 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2105149272"/>
+        <c:crossAx val="-2144380568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1277,15 +1273,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>139700</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>622300</xdr:colOff>
+      <xdr:colOff>596900</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1629,15 +1625,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DE5"/>
+  <dimension ref="A1:DI5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:109">
+    <row r="1" spans="1:113">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1677,296 +1673,296 @@
       <c r="M1">
         <v>11</v>
       </c>
-      <c r="N1">
+      <c r="O1">
         <v>12</v>
       </c>
-      <c r="O1">
+      <c r="P1">
         <v>13</v>
       </c>
-      <c r="P1">
+      <c r="Q1">
         <v>14</v>
       </c>
-      <c r="Q1">
+      <c r="R1">
         <v>15</v>
       </c>
-      <c r="R1">
+      <c r="S1">
         <v>16</v>
       </c>
-      <c r="S1">
+      <c r="T1">
         <v>17</v>
       </c>
-      <c r="T1">
+      <c r="U1">
         <v>18</v>
       </c>
-      <c r="U1">
+      <c r="V1">
         <v>19</v>
       </c>
-      <c r="V1">
+      <c r="W1">
         <v>20</v>
       </c>
-      <c r="W1">
+      <c r="X1">
         <v>21</v>
       </c>
-      <c r="X1">
+      <c r="Y1">
         <v>22</v>
       </c>
-      <c r="Y1">
+      <c r="Z1">
         <v>23</v>
       </c>
-      <c r="Z1">
+      <c r="AA1">
         <v>24</v>
       </c>
-      <c r="AA1">
+      <c r="AB1">
         <v>25</v>
       </c>
-      <c r="AB1">
+      <c r="AC1">
         <v>26</v>
       </c>
-      <c r="AC1">
+      <c r="AD1">
         <v>27</v>
       </c>
-      <c r="AD1">
+      <c r="AE1">
         <v>28</v>
       </c>
-      <c r="AE1">
+      <c r="AG1">
         <v>29</v>
       </c>
-      <c r="AF1">
+      <c r="AH1">
         <v>30</v>
       </c>
-      <c r="AG1">
+      <c r="AI1">
         <v>31</v>
       </c>
-      <c r="AH1">
+      <c r="AJ1">
         <v>32</v>
       </c>
-      <c r="AI1">
+      <c r="AK1">
         <v>33</v>
       </c>
-      <c r="AJ1">
+      <c r="AL1">
         <v>34</v>
       </c>
-      <c r="AK1">
+      <c r="AM1">
         <v>35</v>
       </c>
-      <c r="AL1">
+      <c r="AN1">
         <v>36</v>
       </c>
-      <c r="AM1">
+      <c r="AO1">
         <v>37</v>
       </c>
-      <c r="AN1">
+      <c r="AP1">
         <v>38</v>
       </c>
-      <c r="AO1">
+      <c r="AQ1">
         <v>39</v>
       </c>
-      <c r="AP1">
+      <c r="AR1">
         <v>40</v>
       </c>
-      <c r="AQ1">
+      <c r="AS1">
         <v>41</v>
       </c>
-      <c r="AR1">
+      <c r="AT1">
         <v>42</v>
       </c>
-      <c r="AS1">
+      <c r="AU1">
         <v>43</v>
       </c>
-      <c r="AT1">
+      <c r="AV1">
         <v>44</v>
       </c>
-      <c r="AU1">
+      <c r="AW1">
         <v>45</v>
       </c>
-      <c r="AV1">
+      <c r="AX1">
         <v>46</v>
       </c>
-      <c r="AW1">
+      <c r="AY1">
         <v>47</v>
       </c>
-      <c r="AX1">
+      <c r="AZ1">
         <v>48</v>
       </c>
-      <c r="AY1">
+      <c r="BA1">
         <v>49</v>
       </c>
-      <c r="AZ1">
+      <c r="BB1">
         <v>50</v>
       </c>
-      <c r="BA1">
+      <c r="BC1">
         <v>51</v>
       </c>
-      <c r="BB1">
+      <c r="BD1">
         <v>52</v>
       </c>
-      <c r="BC1">
+      <c r="BE1">
         <v>53</v>
       </c>
-      <c r="BD1">
+      <c r="BG1">
         <v>54</v>
       </c>
-      <c r="BE1">
+      <c r="BH1">
         <v>55</v>
       </c>
-      <c r="BF1">
+      <c r="BI1">
         <v>56</v>
       </c>
-      <c r="BG1">
+      <c r="BJ1">
         <v>57</v>
       </c>
-      <c r="BH1">
+      <c r="BK1">
         <v>58</v>
       </c>
-      <c r="BI1">
+      <c r="BL1">
         <v>59</v>
       </c>
-      <c r="BJ1">
+      <c r="BM1">
         <v>60</v>
       </c>
-      <c r="BK1">
+      <c r="BN1">
         <v>61</v>
       </c>
-      <c r="BL1">
+      <c r="BO1">
         <v>62</v>
       </c>
-      <c r="BM1">
+      <c r="BP1">
         <v>63</v>
       </c>
-      <c r="BN1">
+      <c r="BQ1">
         <v>64</v>
       </c>
-      <c r="BO1">
+      <c r="BR1">
         <v>65</v>
       </c>
-      <c r="BP1">
+      <c r="BS1">
         <v>66</v>
       </c>
-      <c r="BQ1">
+      <c r="BT1">
         <v>67</v>
       </c>
-      <c r="BR1">
+      <c r="BU1">
         <v>68</v>
       </c>
-      <c r="BS1">
+      <c r="BV1">
         <v>69</v>
       </c>
-      <c r="BT1">
+      <c r="BW1">
         <v>70</v>
       </c>
-      <c r="BU1">
+      <c r="BX1">
         <v>71</v>
       </c>
-      <c r="BV1">
+      <c r="BY1">
         <v>72</v>
       </c>
-      <c r="BW1">
+      <c r="BZ1">
         <v>73</v>
       </c>
-      <c r="BX1">
+      <c r="CB1">
         <v>74</v>
       </c>
-      <c r="BY1">
+      <c r="CC1">
         <v>75</v>
       </c>
-      <c r="BZ1">
+      <c r="CD1">
         <v>76</v>
       </c>
-      <c r="CA1">
+      <c r="CE1">
         <v>77</v>
       </c>
-      <c r="CB1">
+      <c r="CF1">
         <v>78</v>
       </c>
-      <c r="CC1">
+      <c r="CG1">
         <v>79</v>
       </c>
-      <c r="CD1">
-        <v>80</v>
-      </c>
-      <c r="CE1">
+      <c r="CH1">
+        <v>80</v>
+      </c>
+      <c r="CI1">
         <v>81</v>
       </c>
-      <c r="CF1">
-        <v>82</v>
-      </c>
-      <c r="CG1">
+      <c r="CJ1">
+        <v>82</v>
+      </c>
+      <c r="CK1">
         <v>83</v>
       </c>
-      <c r="CH1">
+      <c r="CL1">
         <v>84</v>
       </c>
-      <c r="CI1">
+      <c r="CM1">
         <v>85</v>
       </c>
-      <c r="CJ1">
+      <c r="CN1">
         <v>86</v>
       </c>
-      <c r="CK1">
+      <c r="CO1">
         <v>87</v>
       </c>
-      <c r="CL1">
+      <c r="CP1">
         <v>88</v>
       </c>
-      <c r="CM1">
+      <c r="CQ1">
         <v>89</v>
       </c>
-      <c r="CN1">
+      <c r="CR1">
         <v>90</v>
       </c>
-      <c r="CO1">
+      <c r="CS1">
         <v>91</v>
       </c>
-      <c r="CP1">
+      <c r="CT1">
         <v>92</v>
       </c>
-      <c r="CQ1">
+      <c r="CU1">
         <v>93</v>
       </c>
-      <c r="CR1">
+      <c r="CV1">
         <v>94</v>
       </c>
-      <c r="CS1">
+      <c r="CW1">
         <v>95</v>
       </c>
-      <c r="CT1">
+      <c r="CX1">
         <v>96</v>
       </c>
-      <c r="CU1">
+      <c r="CY1">
         <v>97</v>
       </c>
-      <c r="CV1">
+      <c r="CZ1">
         <v>98</v>
       </c>
-      <c r="CW1">
+      <c r="DA1">
         <v>99</v>
       </c>
-      <c r="CX1">
+      <c r="DB1">
         <v>100</v>
       </c>
-      <c r="CY1">
+      <c r="DC1">
         <v>101</v>
       </c>
-      <c r="CZ1">
+      <c r="DD1">
         <v>102</v>
       </c>
-      <c r="DA1">
+      <c r="DE1">
         <v>103</v>
       </c>
-      <c r="DB1">
+      <c r="DF1">
         <v>104</v>
       </c>
-      <c r="DC1">
+      <c r="DG1">
         <v>105</v>
       </c>
-      <c r="DD1">
+      <c r="DH1">
         <v>106</v>
       </c>
-      <c r="DE1">
+      <c r="DI1">
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:109">
+    <row r="2" spans="1:113">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2006,296 +2002,296 @@
       <c r="M2" t="s">
         <v>14</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>15</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>16</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>17</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>18</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>19</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>20</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>21</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>22</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>23</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>24</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>25</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>26</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>27</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>28</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>29</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>30</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AE2" t="s">
         <v>31</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AG2" t="s">
         <v>32</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AH2" t="s">
         <v>33</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AI2" t="s">
         <v>34</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AJ2" t="s">
         <v>35</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AK2" t="s">
         <v>36</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AL2" t="s">
         <v>37</v>
       </c>
-      <c r="AK2" t="s">
+      <c r="AM2" t="s">
         <v>38</v>
       </c>
-      <c r="AL2" t="s">
+      <c r="AN2" t="s">
         <v>39</v>
       </c>
-      <c r="AM2" t="s">
+      <c r="AO2" t="s">
         <v>40</v>
       </c>
-      <c r="AN2" t="s">
+      <c r="AP2" t="s">
         <v>41</v>
       </c>
-      <c r="AO2" t="s">
+      <c r="AQ2" t="s">
         <v>42</v>
       </c>
-      <c r="AP2" t="s">
+      <c r="AR2" t="s">
         <v>43</v>
       </c>
-      <c r="AQ2" t="s">
+      <c r="AS2" t="s">
         <v>44</v>
       </c>
-      <c r="AR2" t="s">
+      <c r="AT2" t="s">
         <v>45</v>
       </c>
-      <c r="AS2" t="s">
+      <c r="AU2" t="s">
         <v>46</v>
       </c>
-      <c r="AT2" t="s">
+      <c r="AV2" t="s">
         <v>47</v>
       </c>
-      <c r="AU2" t="s">
+      <c r="AW2" t="s">
         <v>48</v>
       </c>
-      <c r="AV2" t="s">
+      <c r="AX2" t="s">
         <v>49</v>
       </c>
-      <c r="AW2" t="s">
+      <c r="AY2" t="s">
         <v>50</v>
       </c>
-      <c r="AX2" t="s">
+      <c r="AZ2" t="s">
         <v>51</v>
       </c>
-      <c r="AY2" t="s">
+      <c r="BA2" t="s">
         <v>52</v>
       </c>
-      <c r="AZ2" t="s">
+      <c r="BB2" t="s">
         <v>53</v>
       </c>
-      <c r="BA2" t="s">
+      <c r="BC2" t="s">
         <v>54</v>
       </c>
-      <c r="BB2" t="s">
+      <c r="BD2" t="s">
         <v>55</v>
       </c>
-      <c r="BC2" t="s">
+      <c r="BE2" t="s">
         <v>56</v>
       </c>
-      <c r="BD2" t="s">
+      <c r="BG2" t="s">
         <v>57</v>
       </c>
-      <c r="BE2" t="s">
+      <c r="BH2" t="s">
         <v>58</v>
       </c>
-      <c r="BF2" t="s">
+      <c r="BI2" t="s">
         <v>59</v>
       </c>
-      <c r="BG2" t="s">
+      <c r="BJ2" t="s">
         <v>60</v>
       </c>
-      <c r="BH2" t="s">
+      <c r="BK2" t="s">
         <v>61</v>
       </c>
-      <c r="BI2" t="s">
+      <c r="BL2" t="s">
         <v>62</v>
       </c>
-      <c r="BJ2" t="s">
+      <c r="BM2" t="s">
         <v>63</v>
       </c>
-      <c r="BK2" t="s">
+      <c r="BN2" t="s">
         <v>64</v>
       </c>
-      <c r="BL2" t="s">
+      <c r="BO2" t="s">
         <v>65</v>
       </c>
-      <c r="BM2" t="s">
+      <c r="BP2" t="s">
         <v>66</v>
       </c>
-      <c r="BN2" t="s">
+      <c r="BQ2" t="s">
         <v>67</v>
       </c>
-      <c r="BO2" t="s">
+      <c r="BR2" t="s">
         <v>68</v>
       </c>
-      <c r="BP2" t="s">
+      <c r="BS2" t="s">
         <v>69</v>
       </c>
-      <c r="BQ2" t="s">
+      <c r="BT2" t="s">
         <v>70</v>
       </c>
-      <c r="BR2" t="s">
+      <c r="BU2" t="s">
         <v>71</v>
       </c>
-      <c r="BS2" t="s">
+      <c r="BV2" t="s">
         <v>72</v>
       </c>
-      <c r="BT2" t="s">
+      <c r="BW2" t="s">
         <v>73</v>
       </c>
-      <c r="BU2" t="s">
+      <c r="BX2" t="s">
         <v>74</v>
       </c>
-      <c r="BV2" t="s">
+      <c r="BY2" t="s">
         <v>75</v>
       </c>
-      <c r="BW2" t="s">
+      <c r="BZ2" t="s">
         <v>76</v>
       </c>
-      <c r="BX2" t="s">
+      <c r="CB2" t="s">
         <v>83</v>
       </c>
-      <c r="BY2" t="s">
+      <c r="CC2" t="s">
         <v>84</v>
       </c>
-      <c r="BZ2" t="s">
+      <c r="CD2" t="s">
         <v>85</v>
       </c>
-      <c r="CA2" t="s">
+      <c r="CE2" t="s">
         <v>86</v>
       </c>
-      <c r="CB2" t="s">
+      <c r="CF2" t="s">
         <v>87</v>
       </c>
-      <c r="CC2" t="s">
+      <c r="CG2" t="s">
         <v>88</v>
       </c>
-      <c r="CD2" t="s">
+      <c r="CH2" t="s">
         <v>89</v>
       </c>
-      <c r="CE2" t="s">
+      <c r="CI2" t="s">
         <v>90</v>
       </c>
-      <c r="CF2" t="s">
+      <c r="CJ2" t="s">
         <v>91</v>
       </c>
-      <c r="CG2" t="s">
+      <c r="CK2" t="s">
         <v>92</v>
       </c>
-      <c r="CH2" t="s">
+      <c r="CL2" t="s">
         <v>93</v>
       </c>
-      <c r="CI2" t="s">
+      <c r="CM2" t="s">
         <v>94</v>
       </c>
-      <c r="CJ2" t="s">
+      <c r="CN2" t="s">
         <v>95</v>
       </c>
-      <c r="CK2" t="s">
+      <c r="CO2" t="s">
         <v>96</v>
       </c>
-      <c r="CL2" t="s">
+      <c r="CP2" t="s">
         <v>97</v>
       </c>
-      <c r="CM2" t="s">
+      <c r="CQ2" t="s">
         <v>98</v>
       </c>
-      <c r="CN2" t="s">
+      <c r="CR2" t="s">
         <v>99</v>
       </c>
-      <c r="CO2" t="s">
+      <c r="CS2" t="s">
         <v>100</v>
       </c>
-      <c r="CP2" t="s">
+      <c r="CT2" t="s">
         <v>101</v>
       </c>
-      <c r="CQ2" t="s">
+      <c r="CU2" t="s">
         <v>102</v>
       </c>
-      <c r="CR2" t="s">
+      <c r="CV2" t="s">
         <v>103</v>
       </c>
-      <c r="CS2" t="s">
+      <c r="CW2" t="s">
         <v>104</v>
       </c>
-      <c r="CT2" t="s">
+      <c r="CX2" t="s">
         <v>105</v>
       </c>
-      <c r="CU2" t="s">
+      <c r="CY2" t="s">
         <v>106</v>
       </c>
-      <c r="CV2" t="s">
+      <c r="CZ2" t="s">
         <v>107</v>
       </c>
-      <c r="CW2" t="s">
+      <c r="DA2" t="s">
         <v>108</v>
       </c>
-      <c r="CX2" t="s">
+      <c r="DB2" t="s">
         <v>109</v>
       </c>
-      <c r="CY2" t="s">
+      <c r="DC2" t="s">
         <v>110</v>
       </c>
-      <c r="CZ2" t="s">
+      <c r="DD2" t="s">
         <v>111</v>
       </c>
-      <c r="DA2" t="s">
+      <c r="DE2" t="s">
         <v>112</v>
       </c>
-      <c r="DB2" t="s">
+      <c r="DF2" t="s">
         <v>113</v>
       </c>
-      <c r="DC2" t="s">
+      <c r="DG2" t="s">
         <v>114</v>
       </c>
-      <c r="DD2" t="s">
+      <c r="DH2" t="s">
         <v>115</v>
       </c>
-      <c r="DE2" t="s">
+      <c r="DI2" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="3" spans="1:109">
+    <row r="3" spans="1:113">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -2335,29 +2331,26 @@
       <c r="M3">
         <v>132</v>
       </c>
-      <c r="N3">
-        <v>72</v>
-      </c>
       <c r="O3">
         <v>72</v>
       </c>
       <c r="P3">
+        <v>72</v>
+      </c>
+      <c r="Q3">
         <v>78</v>
       </c>
-      <c r="Q3">
-        <v>80</v>
-      </c>
       <c r="R3">
+        <v>80</v>
+      </c>
+      <c r="S3">
         <v>84</v>
-      </c>
-      <c r="S3">
-        <v>92</v>
       </c>
       <c r="T3">
         <v>92</v>
       </c>
       <c r="U3">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="V3">
         <v>96</v>
@@ -2369,135 +2362,129 @@
         <v>96</v>
       </c>
       <c r="Y3">
+        <v>96</v>
+      </c>
+      <c r="Z3">
         <v>104</v>
       </c>
-      <c r="Z3">
-        <f>Z5*2</f>
+      <c r="AA3">
+        <f>AA5*2</f>
         <v>160</v>
       </c>
-      <c r="AA3">
-        <f t="shared" ref="AA3:AD3" si="0">AA5*2</f>
+      <c r="AB3">
+        <f t="shared" ref="AB3:AE3" si="0">AB5*2</f>
         <v>152</v>
       </c>
-      <c r="AB3">
+      <c r="AC3">
         <f t="shared" si="0"/>
         <v>160</v>
       </c>
-      <c r="AC3">
+      <c r="AD3">
         <f t="shared" si="0"/>
         <v>184</v>
       </c>
-      <c r="AD3">
+      <c r="AE3">
         <f t="shared" si="0"/>
         <v>192</v>
       </c>
-      <c r="AE3">
-        <v>66</v>
-      </c>
-      <c r="AF3">
-        <v>66</v>
-      </c>
       <c r="AG3">
         <v>66</v>
       </c>
       <c r="AH3">
+        <v>66</v>
+      </c>
+      <c r="AI3">
+        <v>66</v>
+      </c>
+      <c r="AJ3">
         <v>72</v>
       </c>
-      <c r="AI3">
+      <c r="AK3">
         <v>72</v>
       </c>
-      <c r="AJ3">
-        <v>80</v>
-      </c>
-      <c r="AK3">
+      <c r="AL3">
+        <v>80</v>
+      </c>
+      <c r="AM3">
         <v>84</v>
       </c>
-      <c r="AL3">
+      <c r="AN3">
         <v>88</v>
       </c>
-      <c r="AM3">
+      <c r="AO3">
         <v>92</v>
       </c>
-      <c r="AN3">
+      <c r="AP3">
         <v>96</v>
       </c>
-      <c r="AO3">
+      <c r="AQ3">
         <v>100</v>
       </c>
-      <c r="AP3">
+      <c r="AR3">
         <v>100</v>
       </c>
-      <c r="AQ3">
+      <c r="AS3">
         <v>104</v>
       </c>
-      <c r="AR3">
-        <f t="shared" ref="AR3:BC3" si="1">AR5*2</f>
+      <c r="AT3">
+        <f t="shared" ref="AT3:BE3" si="1">AT5*2</f>
         <v>152</v>
       </c>
-      <c r="AS3">
+      <c r="AU3">
         <f t="shared" si="1"/>
         <v>168</v>
       </c>
-      <c r="AT3">
+      <c r="AV3">
         <f t="shared" si="1"/>
         <v>184</v>
       </c>
-      <c r="AU3">
+      <c r="AW3">
         <f t="shared" si="1"/>
         <v>192</v>
       </c>
-      <c r="AV3">
+      <c r="AX3">
         <f t="shared" si="1"/>
         <v>192</v>
       </c>
-      <c r="AW3">
+      <c r="AY3">
         <f t="shared" si="1"/>
         <v>208</v>
       </c>
-      <c r="AX3">
+      <c r="AZ3">
         <f t="shared" si="1"/>
         <v>208</v>
       </c>
-      <c r="AY3">
+      <c r="BA3">
         <f t="shared" si="1"/>
         <v>216</v>
       </c>
-      <c r="AZ3">
+      <c r="BB3">
         <f t="shared" si="1"/>
         <v>216</v>
       </c>
-      <c r="BA3">
+      <c r="BC3">
         <f t="shared" si="1"/>
         <v>224</v>
       </c>
-      <c r="BB3">
+      <c r="BD3">
         <f t="shared" si="1"/>
         <v>224</v>
       </c>
-      <c r="BC3">
+      <c r="BE3">
         <f t="shared" si="1"/>
         <v>232</v>
       </c>
-      <c r="BD3">
+      <c r="BG3">
         <v>60</v>
       </c>
-      <c r="BE3">
+      <c r="BH3">
         <v>63</v>
       </c>
-      <c r="BF3">
+      <c r="BI3">
         <v>69</v>
       </c>
-      <c r="BG3">
+      <c r="BJ3">
         <v>72</v>
-      </c>
-      <c r="BH3">
-        <v>76</v>
-      </c>
-      <c r="BI3">
-        <v>76</v>
-      </c>
-      <c r="BJ3">
-        <v>76</v>
       </c>
       <c r="BK3">
         <v>76</v>
@@ -2509,76 +2496,73 @@
         <v>76</v>
       </c>
       <c r="BN3">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="BO3">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="BP3">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="BQ3">
+        <v>80</v>
+      </c>
+      <c r="BR3">
+        <v>80</v>
+      </c>
+      <c r="BS3">
+        <v>80</v>
+      </c>
+      <c r="BT3">
         <v>84</v>
       </c>
-      <c r="BR3">
+      <c r="BU3">
         <v>88</v>
       </c>
-      <c r="BS3">
+      <c r="BV3">
         <v>96</v>
       </c>
-      <c r="BT3">
+      <c r="BW3">
         <v>100</v>
       </c>
-      <c r="BU3">
+      <c r="BX3">
         <v>104</v>
       </c>
-      <c r="BV3">
+      <c r="BY3">
         <v>108</v>
       </c>
-      <c r="BW3">
+      <c r="BZ3">
         <v>126</v>
       </c>
-      <c r="BX3">
+      <c r="CB3">
         <v>60</v>
       </c>
-      <c r="BY3">
+      <c r="CC3">
         <v>63</v>
       </c>
-      <c r="BZ3">
+      <c r="CD3">
         <v>63</v>
       </c>
-      <c r="CA3">
+      <c r="CE3">
         <v>66</v>
       </c>
-      <c r="CB3">
+      <c r="CF3">
         <v>66</v>
       </c>
-      <c r="CC3">
+      <c r="CG3">
         <v>69</v>
       </c>
-      <c r="CD3">
+      <c r="CH3">
         <v>69</v>
       </c>
-      <c r="CE3">
+      <c r="CI3">
         <v>69</v>
       </c>
-      <c r="CF3">
+      <c r="CJ3">
         <v>72</v>
       </c>
-      <c r="CG3">
+      <c r="CK3">
         <v>72</v>
-      </c>
-      <c r="CH3">
-        <v>76</v>
-      </c>
-      <c r="CI3">
-        <v>76</v>
-      </c>
-      <c r="CJ3">
-        <v>76</v>
-      </c>
-      <c r="CK3">
-        <v>76</v>
       </c>
       <c r="CL3">
         <v>76</v>
@@ -2599,56 +2583,68 @@
         <v>76</v>
       </c>
       <c r="CR3">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="CS3">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="CT3">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="CU3">
+        <v>76</v>
+      </c>
+      <c r="CV3">
+        <v>80</v>
+      </c>
+      <c r="CW3">
+        <v>80</v>
+      </c>
+      <c r="CX3">
+        <v>80</v>
+      </c>
+      <c r="CY3">
         <v>84</v>
       </c>
-      <c r="CV3">
+      <c r="CZ3">
         <v>92</v>
       </c>
-      <c r="CW3">
+      <c r="DA3">
         <v>92</v>
       </c>
-      <c r="CX3">
+      <c r="DB3">
         <v>92</v>
       </c>
-      <c r="CY3">
-        <f t="shared" ref="CY3:DE3" si="2">CY5*2</f>
+      <c r="DC3">
+        <f t="shared" ref="DC3:DI3" si="2">DC5*2</f>
         <v>138</v>
       </c>
-      <c r="CZ3">
+      <c r="DD3">
         <f t="shared" si="2"/>
         <v>138</v>
       </c>
-      <c r="DA3">
+      <c r="DE3">
         <f t="shared" si="2"/>
         <v>156</v>
       </c>
-      <c r="DB3">
+      <c r="DF3">
         <f t="shared" si="2"/>
         <v>180</v>
       </c>
-      <c r="DC3">
+      <c r="DG3">
         <f t="shared" si="2"/>
         <v>198</v>
       </c>
-      <c r="DD3">
+      <c r="DH3">
         <f t="shared" si="2"/>
         <v>206</v>
       </c>
-      <c r="DE3">
+      <c r="DI3">
         <f t="shared" si="2"/>
         <v>216</v>
       </c>
     </row>
-    <row r="4" spans="1:109">
+    <row r="4" spans="1:113">
       <c r="A4" t="s">
         <v>77</v>
       </c>
@@ -2688,9 +2684,6 @@
       <c r="M4" t="s">
         <v>78</v>
       </c>
-      <c r="N4" t="s">
-        <v>79</v>
-      </c>
       <c r="O4" t="s">
         <v>79</v>
       </c>
@@ -2740,10 +2733,7 @@
         <v>79</v>
       </c>
       <c r="AE4" t="s">
-        <v>80</v>
-      </c>
-      <c r="AF4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AG4" t="s">
         <v>80</v>
@@ -2815,13 +2805,10 @@
         <v>80</v>
       </c>
       <c r="BD4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="BE4" t="s">
-        <v>81</v>
-      </c>
-      <c r="BF4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="BG4" t="s">
         <v>81</v>
@@ -2875,16 +2862,13 @@
         <v>81</v>
       </c>
       <c r="BX4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="BY4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="BZ4" t="s">
-        <v>82</v>
-      </c>
-      <c r="CA4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="CB4" t="s">
         <v>82</v>
@@ -2976,78 +2960,90 @@
       <c r="DE4" t="s">
         <v>82</v>
       </c>
+      <c r="DF4" t="s">
+        <v>82</v>
+      </c>
+      <c r="DG4" t="s">
+        <v>82</v>
+      </c>
+      <c r="DH4" t="s">
+        <v>82</v>
+      </c>
+      <c r="DI4" t="s">
+        <v>82</v>
+      </c>
     </row>
-    <row r="5" spans="1:109">
-      <c r="Z5">
-        <v>80</v>
-      </c>
+    <row r="5" spans="1:113">
       <c r="AA5">
+        <v>80</v>
+      </c>
+      <c r="AB5">
         <v>76</v>
       </c>
-      <c r="AB5">
-        <v>80</v>
-      </c>
       <c r="AC5">
+        <v>80</v>
+      </c>
+      <c r="AD5">
         <v>92</v>
       </c>
-      <c r="AD5">
+      <c r="AE5">
         <v>96</v>
       </c>
-      <c r="AR5">
+      <c r="AT5">
         <v>76</v>
       </c>
-      <c r="AS5">
+      <c r="AU5">
         <v>84</v>
       </c>
-      <c r="AT5">
+      <c r="AV5">
         <v>92</v>
       </c>
-      <c r="AU5">
+      <c r="AW5">
         <v>96</v>
       </c>
-      <c r="AV5">
+      <c r="AX5">
         <v>96</v>
       </c>
-      <c r="AW5">
+      <c r="AY5">
         <v>104</v>
       </c>
-      <c r="AX5">
+      <c r="AZ5">
         <v>104</v>
       </c>
-      <c r="AY5">
+      <c r="BA5">
         <v>108</v>
       </c>
-      <c r="AZ5">
+      <c r="BB5">
         <v>108</v>
       </c>
-      <c r="BA5">
+      <c r="BC5">
         <v>112</v>
       </c>
-      <c r="BB5">
+      <c r="BD5">
         <v>112</v>
       </c>
-      <c r="BC5">
+      <c r="BE5">
         <v>116</v>
       </c>
-      <c r="CY5">
+      <c r="DC5">
         <v>69</v>
       </c>
-      <c r="CZ5">
+      <c r="DD5">
         <v>69</v>
       </c>
-      <c r="DA5">
+      <c r="DE5">
         <v>78</v>
       </c>
-      <c r="DB5">
+      <c r="DF5">
         <v>90</v>
       </c>
-      <c r="DC5">
+      <c r="DG5">
         <v>99</v>
       </c>
-      <c r="DD5">
+      <c r="DH5">
         <v>103</v>
       </c>
-      <c r="DE5">
+      <c r="DI5">
         <v>108</v>
       </c>
     </row>

</xml_diff>